<commit_message>
preparation of meeting with Ronald and Apo
</commit_message>
<xml_diff>
--- a/DGA1031/Book1.xlsx
+++ b/DGA1031/Book1.xlsx
@@ -214,12 +214,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -504,13 +505,13 @@
   <dimension ref="A1:AB49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16:XFD25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
     <col min="3" max="3" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="28" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -671,10 +672,10 @@
       <c r="AB7" s="2"/>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5"/>
+      <c r="B8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
@@ -703,10 +704,10 @@
       <c r="AB8" s="2"/>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5"/>
+      <c r="B9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
@@ -735,11 +736,11 @@
       <c r="AB9" s="2"/>
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
@@ -768,10 +769,10 @@
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="5"/>
+      <c r="C11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
       <c r="F11" s="2"/>

</xml_diff>